<commit_message>
Ajustes de actas y envio ftp
</commit_message>
<xml_diff>
--- a/temp_excel_file.xlsx
+++ b/temp_excel_file.xlsx
@@ -308,10 +308,10 @@
     <t/>
   </si>
   <si>
-    <t>JORGE FRANKLYN COAQUIRA RAMOS</t>
-  </si>
-  <si>
-    <t>jcoaquirar@pj.gob.pe</t>
+    <t>ALEXANDER CHRISTIAN FLORES CASTILLO</t>
+  </si>
+  <si>
+    <t>aflorescast@pj.gob.pe</t>
   </si>
   <si>
     <t>CONTROL PATRIMONIAL</t>
@@ -320,37 +320,37 @@
     <t>PALACIO DE JUSTICIA</t>
   </si>
   <si>
-    <t>AV SIGLO XX S/N</t>
-  </si>
-  <si>
-    <t>47087903</t>
+    <t>AV. SIGLO XX S/N</t>
+  </si>
+  <si>
+    <t>76639137</t>
   </si>
   <si>
     <t>31-12-2024</t>
   </si>
   <si>
-    <t>ASIGNACIÓN</t>
-  </si>
-  <si>
-    <t>2-2024</t>
-  </si>
-  <si>
-    <t>740899500002</t>
-  </si>
-  <si>
-    <t>UNIDAD CENTRAL DE PROCESO - CPU</t>
-  </si>
-  <si>
-    <t>LENOVO</t>
-  </si>
-  <si>
-    <t>THINKCENTER M920S</t>
+    <t>DEVOLUCIÓN</t>
+  </si>
+  <si>
+    <t>1-2024</t>
+  </si>
+  <si>
+    <t>740800010005</t>
+  </si>
+  <si>
+    <t>IMPRESORA DE CHEQUES</t>
+  </si>
+  <si>
+    <t>DELL</t>
+  </si>
+  <si>
+    <t>OptiPlex 3060</t>
   </si>
   <si>
     <t>NEGRO</t>
   </si>
   <si>
-    <t>ASDERT</t>
+    <t>HTHNBNN</t>
   </si>
 </sst>
 </file>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="14" spans="1:9" ht="14.25" customHeight="true">
       <c r="A14" s="13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Implementacion para persistir versiones de bienes
</commit_message>
<xml_diff>
--- a/temp_excel_file.xlsx
+++ b/temp_excel_file.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="58">
   <si>
     <r>
       <rPr>
@@ -308,10 +308,10 @@
     <t/>
   </si>
   <si>
-    <t>ALEXANDER CHRISTIAN FLORES CASTILLO</t>
-  </si>
-  <si>
-    <t>aflorescast@pj.gob.pe</t>
+    <t>JORGE FRANKLYN COAQUIRA RAMOS</t>
+  </si>
+  <si>
+    <t>jcoaquirar@pj.gob.pe</t>
   </si>
   <si>
     <t>CONTROL PATRIMONIAL</t>
@@ -323,34 +323,31 @@
     <t>AV. SIGLO XX S/N</t>
   </si>
   <si>
-    <t>76639137</t>
-  </si>
-  <si>
-    <t>31-12-2024</t>
-  </si>
-  <si>
-    <t>DEVOLUCIÓN</t>
-  </si>
-  <si>
-    <t>1-2024</t>
-  </si>
-  <si>
-    <t>740800010005</t>
+    <t>47087903</t>
+  </si>
+  <si>
+    <t>02-01-2025</t>
+  </si>
+  <si>
+    <t>ASIGNACIÓN</t>
+  </si>
+  <si>
+    <t>7-2025</t>
+  </si>
+  <si>
+    <t>740800010013</t>
   </si>
   <si>
     <t>IMPRESORA DE CHEQUES</t>
   </si>
   <si>
-    <t>DELL</t>
-  </si>
-  <si>
-    <t>OptiPlex 3060</t>
-  </si>
-  <si>
-    <t>NEGRO</t>
-  </si>
-  <si>
-    <t>HTHNBNN</t>
+    <t>S/M</t>
+  </si>
+  <si>
+    <t>GRIS</t>
+  </si>
+  <si>
+    <t>GFDFGH</t>
   </si>
 </sst>
 </file>
@@ -1387,13 +1384,13 @@
         <v>55</v>
       </c>
       <c r="E14" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="G14" s="15" t="s">
         <v>57</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>58</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="14" t="s">

</xml_diff>